<commit_message>
add script p/ agregar puntajes a la base de datos
</commit_message>
<xml_diff>
--- a/planteles.xlsx
+++ b/planteles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\granDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\granDTcalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B77B6B-D50F-4C96-AE57-9E50B004B4EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CA1759-C60C-4819-9C4F-798BEE94C08B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="876">
   <si>
     <t>Assmann, Fabián</t>
   </si>
@@ -2648,6 +2648,12 @@
   </si>
   <si>
     <t>De La Fuente, Hernán</t>
+  </si>
+  <si>
+    <t>González, Matías N.</t>
+  </si>
+  <si>
+    <t>Rodríguez, Lucas A.</t>
   </si>
 </sst>
 </file>
@@ -3013,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O799"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="A307" sqref="A307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13352,7 +13358,7 @@
     </row>
     <row r="306" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>321</v>
+        <v>875</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>330</v>
@@ -15685,7 +15691,7 @@
     </row>
     <row r="375" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>152</v>
+        <v>874</v>
       </c>
       <c r="B375" s="1" t="s">
         <v>396</v>

</xml_diff>